<commit_message>
utmb pv pacing chart
</commit_message>
<xml_diff>
--- a/data/utmb_puerto-vallarta100/PuertoVallartaUTMB20220818.xlsx
+++ b/data/utmb_puerto-vallarta100/PuertoVallartaUTMB20220818.xlsx
@@ -8,16 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spak01\Documents\GitHub\ultradata\data\utmb_puerto-vallarta100\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC442D9-A108-42B2-A907-6C2F3EA3B0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665FC3A7-DC01-43E1-83A3-90F297B250C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8805" yWindow="1110" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6780" yWindow="5265" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -626,7 +638,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -926,13 +938,28 @@
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="B10" s="5">
+        <v>1522</v>
+      </c>
+      <c r="C10" s="5">
+        <v>7</v>
+      </c>
+      <c r="D10" s="5">
+        <f>D9+C10</f>
+        <v>69.599999999999994</v>
+      </c>
+      <c r="E10" s="5">
+        <v>2715</v>
+      </c>
+      <c r="F10" s="5">
+        <v>2588</v>
+      </c>
+      <c r="G10" s="7">
+        <v>2.2916666666666669E-2</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0.36736111111111108</v>
+      </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="10"/>
@@ -1363,7 +1390,7 @@
     <row r="34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="82" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="82" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>